<commit_message>
RMS-Messungen wiederholt, OptDSP angefangen, OptARM abgeschlossen
</commit_message>
<xml_diff>
--- a/Results/ResultsExtraktion2.xlsx
+++ b/Results/ResultsExtraktion2.xlsx
@@ -7,21 +7,22 @@
     <workbookView xWindow="0" yWindow="135" windowWidth="14115" windowHeight="13740" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="ARM MCL1" sheetId="1" r:id="rId1"/>
-    <sheet name="ARM MCL 2" sheetId="2" r:id="rId2"/>
-    <sheet name="ARM MCL3" sheetId="3" r:id="rId3"/>
-    <sheet name="ARM MCL4" sheetId="8" r:id="rId4"/>
-    <sheet name="DSP MCL1" sheetId="4" r:id="rId5"/>
-    <sheet name="DSP MCL2" sheetId="5" r:id="rId6"/>
-    <sheet name="DSP MCL3" sheetId="6" r:id="rId7"/>
-    <sheet name="DSP MCL4" sheetId="7" r:id="rId8"/>
+    <sheet name="Feature Überblick" sheetId="9" r:id="rId1"/>
+    <sheet name="ARM MCL1" sheetId="1" r:id="rId2"/>
+    <sheet name="ARM MCL 2" sheetId="2" r:id="rId3"/>
+    <sheet name="ARM MCL3" sheetId="3" r:id="rId4"/>
+    <sheet name="ARM MCL4" sheetId="8" r:id="rId5"/>
+    <sheet name="DSP MCL1" sheetId="4" r:id="rId6"/>
+    <sheet name="DSP MCL2" sheetId="5" r:id="rId7"/>
+    <sheet name="DSP MCL3" sheetId="6" r:id="rId8"/>
+    <sheet name="DSP MCL4" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>DSP</t>
   </si>
@@ -57,9 +58,6 @@
   </si>
   <si>
     <t>MFCC</t>
-  </si>
-  <si>
-    <t>Libav NEON + NEON Opt</t>
   </si>
   <si>
     <t>Gesamt</t>
@@ -105,6 +103,12 @@
   </si>
   <si>
     <t>AOMIC</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>Libav NEON + Handopt.</t>
   </si>
 </sst>
 </file>
@@ -154,7 +158,190 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
-  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Überblick'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Feature Überblick'!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MAG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SF</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MFCC</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>HW</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>NASE</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>OSC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ZCR</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RMS</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LE</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SCF</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SBER</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>CV</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>AOMIC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Überblick'!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.639597834493426E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.848414539829853E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2242846094354215E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4470224284609439E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3201856148491878E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1848414539829853E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3361702127659575E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1299806576402321E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11704448742746615</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9118329466357307E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5290023201856148E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6040216550657389E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.5127610208816705E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3689095127610209E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4795050270688321E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6395978344934262E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="71616000"/>
+        <c:axId val="70471680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="71616000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70471680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70471680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71616000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -162,253 +349,135 @@
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ARM MCL 2'!$A$15</c:f>
+              <c:f>'Feature Überblick'!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FFT</c:v>
+                  <c:v>ARM+NEON</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:f>'Feature Überblick'!$A$22:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MAG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MFCC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ARM MCL 2'!$B$15</c:f>
+              <c:f>'Feature Überblick'!$B$22:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>58.591443634822838</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.31547563805104412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.848414539829853E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.817478731631864E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3361702127659575E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ARM MCL 2'!$A$19</c:f>
+              <c:f>'Feature Überblick'!$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>OSC</c:v>
+                  <c:v>Libav NEON + Handopt.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:f>'Feature Überblick'!$A$22:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MAG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MFCC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HW</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ARM MCL 2'!$B$19</c:f>
+              <c:f>'Feature Überblick'!$C$22:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>21.016511186902193</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.639597834493426E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9110595514307813E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1848414539829853E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9013539651837522E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MAG</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.1032140202690979</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MFCC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.0650097594520815</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>HW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4.1948278377083001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NASE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ARM+NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.0289935608454952</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="48907392"/>
-        <c:axId val="48908928"/>
+        <c:axId val="78333824"/>
+        <c:axId val="78335360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48907392"/>
+        <c:axId val="78333824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="48908928"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78335360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48908928"/>
+        <c:axId val="78335360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +494,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Laufzeitanteil in [%]</a:t>
+                  <a:t>Lauftzeit in [ms/Fenster]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -434,450 +503,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48907392"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1100">
-          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
-    <c:pageSetup orientation="portrait"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FFT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$24:$D$24</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Libav ARM</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Libav VFP</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$25:$D$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1263.3800000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>373.07</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41.96</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="48933504"/>
-        <c:axId val="48943488"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="48933504"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48943488"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="48943488"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Laufzeitmessung in [ms]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48933504"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1100">
-          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>HW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>60.39</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$32</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FFT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>41.96</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MAG</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>102.26</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MFCC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>101.71</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NASE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>29.21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$A$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>OSC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'ARM MCL 2'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Libav NEON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'ARM MCL 2'!$B$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>302.56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="56131968"/>
-        <c:axId val="56133504"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="56131968"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56133504"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="56133504"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Laufzeitmessung in [ms]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56131968"/>
+        <c:crossAx val="78333824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -909,7 +535,830 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>58.591443634822838</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OSC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.016511186902193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.1032140202690979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MFCC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.0650097594520815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.1948278377083001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NASE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARM+NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.0289935608454952</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="75294976"/>
+        <c:axId val="75460608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75294976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="75460608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75460608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Laufzeitanteil in [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75294976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$24:$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Libav ARM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Libav VFP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$25:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1263.3800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>373.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="75476992"/>
+        <c:axId val="75478528"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75476992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75478528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75478528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Laufzeitmessung in [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75476992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>41.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>102.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MFCC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>101.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NASE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>29.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OSC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM MCL 2'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Libav NEON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM MCL 2'!$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>302.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="43094784"/>
+        <c:axId val="43096320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43094784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43096320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43096320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Laufzeitmessung in [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43094784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1289,10 +1738,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="str">
+        <f>'ARM MCL1'!D1</f>
+        <v>ARM+NEON</v>
+      </c>
+      <c r="C1" t="str">
+        <f>'ARM MCL1'!G1</f>
+        <v>Libav NEON</v>
+      </c>
+      <c r="D1" t="str">
+        <f>'ARM MCL1'!H1</f>
+        <v>Libav NEON + Handopt.</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="str">
+        <f>'ARM MCL1'!A2</f>
+        <v>FFT</v>
+      </c>
+      <c r="B2">
+        <f>'ARM MCL1'!D2/1293</f>
+        <v>0.31547563805104412</v>
+      </c>
+      <c r="C2">
+        <f>'ARM MCL1'!G2/1293</f>
+        <v>1.639597834493426E-2</v>
+      </c>
+      <c r="D2">
+        <f>'ARM MCL1'!H2/1293</f>
+        <v>1.639597834493426E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="str">
+        <f>'ARM MCL1'!A3</f>
+        <v>MAG</v>
+      </c>
+      <c r="B3">
+        <f>'ARM MCL1'!D3/1293</f>
+        <v>3.848414539829853E-2</v>
+      </c>
+      <c r="C3">
+        <f>'ARM MCL1'!G3/1293</f>
+        <v>3.848414539829853E-2</v>
+      </c>
+      <c r="D3">
+        <f>'ARM MCL1'!H3/1293</f>
+        <v>1.9110595514307813E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="str">
+        <f>'ARM MCL1'!A4</f>
+        <v>SC</v>
+      </c>
+      <c r="B4">
+        <f>'ARM MCL1'!D4/1293</f>
+        <v>1.2242846094354215E-2</v>
+      </c>
+      <c r="C4">
+        <f>'ARM MCL1'!G4/1293</f>
+        <v>1.2242846094354215E-2</v>
+      </c>
+      <c r="D4">
+        <f>'ARM MCL1'!H4/1293</f>
+        <v>1.2242846094354215E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="str">
+        <f>'ARM MCL1'!A5</f>
+        <v>SR</v>
+      </c>
+      <c r="B5">
+        <f>'ARM MCL1'!D5/1293</f>
+        <v>4.4470224284609439E-3</v>
+      </c>
+      <c r="C5">
+        <f>'ARM MCL1'!G5/1293</f>
+        <v>4.4470224284609439E-3</v>
+      </c>
+      <c r="D5">
+        <f>'ARM MCL1'!H5/1293</f>
+        <v>4.4470224284609439E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="str">
+        <f>'ARM MCL1'!A6</f>
+        <v>SF</v>
+      </c>
+      <c r="B6">
+        <f>'ARM MCL1'!D6/1293</f>
+        <v>2.3201856148491878E-3</v>
+      </c>
+      <c r="C6">
+        <f>'ARM MCL1'!G6/1293</f>
+        <v>2.3201856148491878E-3</v>
+      </c>
+      <c r="D6">
+        <f>'ARM MCL1'!H6/1293</f>
+        <v>2.3201856148491878E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="str">
+        <f>'ARM MCL1'!A7</f>
+        <v>MFCC</v>
+      </c>
+      <c r="B7">
+        <f>'ARM MCL1'!D7/1293</f>
+        <v>3.817478731631864E-2</v>
+      </c>
+      <c r="C7">
+        <f>'ARM MCL1'!G7/1293</f>
+        <v>3.1848414539829853E-2</v>
+      </c>
+      <c r="D7">
+        <f>'ARM MCL1'!H7/1293</f>
+        <v>3.1848414539829853E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="str">
+        <f>'ARM MCL 2'!A2</f>
+        <v>HW</v>
+      </c>
+      <c r="B8">
+        <f>'ARM MCL 2'!D2/2585</f>
+        <v>2.3361702127659575E-2</v>
+      </c>
+      <c r="C8">
+        <f>'ARM MCL 2'!G2/2585</f>
+        <v>2.3361702127659575E-2</v>
+      </c>
+      <c r="D8">
+        <f>'ARM MCL 2'!H2/2585</f>
+        <v>6.9013539651837522E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="str">
+        <f>'ARM MCL 2'!A6</f>
+        <v>NASE</v>
+      </c>
+      <c r="B9">
+        <f>'ARM MCL 2'!D6/2585</f>
+        <v>1.1299806576402321E-2</v>
+      </c>
+      <c r="C9">
+        <f>'ARM MCL 2'!G6/2585</f>
+        <v>1.1299806576402321E-2</v>
+      </c>
+      <c r="D9">
+        <f>'ARM MCL 2'!H6/2585</f>
+        <v>1.1961315280464218E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="str">
+        <f>'ARM MCL 2'!A7</f>
+        <v>OSC</v>
+      </c>
+      <c r="B10">
+        <f>'ARM MCL 2'!D7/2585</f>
+        <v>0.11704448742746615</v>
+      </c>
+      <c r="C10">
+        <f>'ARM MCL 2'!G7/2585</f>
+        <v>0.11704448742746615</v>
+      </c>
+      <c r="D10">
+        <f>'ARM MCL 2'!H7/2585</f>
+        <v>0.11659187620889748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="str">
+        <f>'ARM MCL3'!A2</f>
+        <v>ZCR</v>
+      </c>
+      <c r="B11">
+        <f>'ARM MCL3'!D2/1293</f>
+        <v>3.9118329466357307E-2</v>
+      </c>
+      <c r="C11">
+        <f>'ARM MCL3'!G2/1293</f>
+        <v>3.9118329466357307E-2</v>
+      </c>
+      <c r="D11">
+        <f>'ARM MCL3'!H2/1293</f>
+        <v>3.9118329466357307E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="str">
+        <f>'ARM MCL3'!A3</f>
+        <v>RMS</v>
+      </c>
+      <c r="B12">
+        <f>'ARM MCL3'!D3/1293</f>
+        <v>2.5290023201856148E-3</v>
+      </c>
+      <c r="C12">
+        <f>'ARM MCL3'!G3/1293</f>
+        <v>2.5290023201856148E-3</v>
+      </c>
+      <c r="D12">
+        <f>'ARM MCL3'!H3/1293</f>
+        <v>2.5290023201856148E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="str">
+        <f>'ARM MCL3'!A4</f>
+        <v>LE</v>
+      </c>
+      <c r="B13">
+        <f>'ARM MCL3'!D4/1293</f>
+        <v>3.6040216550657389E-3</v>
+      </c>
+      <c r="C13">
+        <f>'ARM MCL3'!G4/1293</f>
+        <v>3.6040216550657389E-3</v>
+      </c>
+      <c r="D13">
+        <f>'ARM MCL3'!H4/1293</f>
+        <v>3.6040216550657389E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="str">
+        <f>'ARM MCL4'!A4</f>
+        <v>SCF</v>
+      </c>
+      <c r="B14">
+        <f>'ARM MCL4'!D4/1293</f>
+        <v>9.5127610208816705E-4</v>
+      </c>
+      <c r="C14">
+        <f>'ARM MCL4'!G4/1293</f>
+        <v>9.5127610208816705E-4</v>
+      </c>
+      <c r="D14">
+        <f>'ARM MCL4'!H4/1293</f>
+        <v>1.0440835266821347E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="str">
+        <f>'ARM MCL4'!A5</f>
+        <v>SBER</v>
+      </c>
+      <c r="B15">
+        <f>'ARM MCL4'!D5/1293</f>
+        <v>1.3689095127610209E-3</v>
+      </c>
+      <c r="C15">
+        <f>'ARM MCL4'!G5/1293</f>
+        <v>1.3689095127610209E-3</v>
+      </c>
+      <c r="D15">
+        <f>'ARM MCL4'!H5/1293</f>
+        <v>1.4462490332559938E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="str">
+        <f>'ARM MCL4'!A6</f>
+        <v>CV</v>
+      </c>
+      <c r="B16">
+        <f>'ARM MCL4'!D6/1293</f>
+        <v>1.4795050270688321E-2</v>
+      </c>
+      <c r="C16">
+        <f>'ARM MCL4'!G6/1293</f>
+        <v>1.4795050270688321E-2</v>
+      </c>
+      <c r="D16">
+        <f>'ARM MCL4'!H6/1293</f>
+        <v>1.5212683681361177E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="str">
+        <f>'ARM MCL4'!A7</f>
+        <v>AOMIC</v>
+      </c>
+      <c r="B17">
+        <f>'ARM MCL4'!D7/1293</f>
+        <v>1.6395978344934262E-3</v>
+      </c>
+      <c r="C17">
+        <f>'ARM MCL4'!G7/1293</f>
+        <v>1.6395978344934262E-3</v>
+      </c>
+      <c r="D17">
+        <f>'ARM MCL4'!H7/1293</f>
+        <v>1.5313225058004641E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="str">
+        <f>B1</f>
+        <v>ARM+NEON</v>
+      </c>
+      <c r="C21" t="str">
+        <f>D1</f>
+        <v>Libav NEON + Handopt.</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="str">
+        <f>A2</f>
+        <v>FFT</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:C22" si="0">B2</f>
+        <v>0.31547563805104412</v>
+      </c>
+      <c r="C22">
+        <f>D2</f>
+        <v>1.639597834493426E-2</v>
+      </c>
+      <c r="D22">
+        <f>B22/C22</f>
+        <v>19.241037735849059</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="str">
+        <f>A3</f>
+        <v>MAG</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:C23" si="1">B3</f>
+        <v>3.848414539829853E-2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C25" si="2">D3</f>
+        <v>1.9110595514307813E-2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D25" si="3">B23/C23</f>
+        <v>2.0137596114933225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="str">
+        <f>A7</f>
+        <v>MFCC</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:C24" si="4">B7</f>
+        <v>3.817478731631864E-2</v>
+      </c>
+      <c r="C24">
+        <f>D7</f>
+        <v>3.1848414539829853E-2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>1.1986401165614375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="str">
+        <f>A8</f>
+        <v>HW</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:C25" si="5">B8</f>
+        <v>2.3361702127659575E-2</v>
+      </c>
+      <c r="C25">
+        <f>D8</f>
+        <v>6.9013539651837522E-3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>3.385089686098655</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1326,7 +2183,7 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1357,7 +2214,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>691.68</v>
@@ -1383,7 +2240,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>42.27</v>
@@ -1409,7 +2266,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>39.01</v>
@@ -1435,7 +2292,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>20.86</v>
@@ -1482,12 +2339,12 @@
         <v>41.18</v>
       </c>
       <c r="H7">
-        <v>49.36</v>
+        <v>41.18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>
@@ -1515,7 +2372,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>119.85</v>
+        <v>111.66999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1537,12 +2394,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1576,12 +2433,12 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>47.08</v>
@@ -1633,7 +2490,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1384.26</v>
@@ -1685,7 +2542,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>32.590000000000003</v>
@@ -1711,7 +2568,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>351.69</v>
@@ -1737,7 +2594,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>
@@ -1766,6 +2623,12 @@
       <c r="H9">
         <f t="shared" si="0"/>
         <v>524.67000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="C11">
+        <f>D9/H9</f>
+        <v>2.7438771037032796</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1943,12 +2806,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1982,118 +2845,130 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>107.75</v>
+        <v>88.34</v>
       </c>
       <c r="C2">
-        <v>53.97</v>
+        <v>50.53</v>
       </c>
       <c r="D2">
-        <v>52.51</v>
+        <v>50.58</v>
       </c>
       <c r="E2">
-        <v>107.75</v>
+        <f>B2</f>
+        <v>88.34</v>
       </c>
       <c r="F2">
-        <v>53.97</v>
+        <f>C2</f>
+        <v>50.53</v>
       </c>
       <c r="G2">
-        <v>52.51</v>
+        <f>$D$2</f>
+        <v>50.58</v>
       </c>
       <c r="H2">
-        <v>50.36</v>
+        <f>$D$2</f>
+        <v>50.58</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>58.77</v>
+        <v>46.42</v>
       </c>
       <c r="C3">
-        <v>24.91</v>
+        <v>18.04</v>
       </c>
       <c r="D3">
-        <v>3.8</v>
+        <v>3.27</v>
       </c>
       <c r="E3">
-        <v>58.77</v>
+        <f t="shared" ref="E3:E4" si="0">B3</f>
+        <v>46.42</v>
       </c>
       <c r="F3">
-        <v>24.91</v>
+        <f t="shared" ref="F3:F4" si="1">C3</f>
+        <v>18.04</v>
       </c>
       <c r="G3">
-        <v>3.8</v>
+        <f>$D$3</f>
+        <v>3.27</v>
       </c>
       <c r="H3">
-        <v>4.01</v>
+        <f>$D$3</f>
+        <v>3.27</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>9.5299999999999994</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C4">
-        <v>6.57</v>
+        <v>6.71</v>
       </c>
       <c r="D4">
-        <v>4.5999999999999996</v>
+        <v>4.66</v>
       </c>
       <c r="E4">
-        <v>9.5299999999999994</v>
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F4">
-        <v>6.57</v>
+        <f t="shared" si="1"/>
+        <v>6.71</v>
       </c>
       <c r="G4">
-        <v>4.5999999999999996</v>
+        <f>$D$4</f>
+        <v>4.66</v>
       </c>
       <c r="H4">
-        <v>4.83</v>
+        <f>$D$4</f>
+        <v>4.66</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <f>SUM(B2:B4)</f>
-        <v>176.05</v>
+        <v>143.95999999999998</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:H6" si="0">SUM(C2:C4)</f>
-        <v>85.449999999999989</v>
+        <f t="shared" ref="C6:H6" si="2">SUM(C2:C4)</f>
+        <v>75.279999999999987</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>60.91</v>
+        <f t="shared" si="2"/>
+        <v>58.510000000000005</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>176.05</v>
+        <f t="shared" si="2"/>
+        <v>143.95999999999998</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>85.449999999999989</v>
+        <f t="shared" si="2"/>
+        <v>75.279999999999987</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>60.91</v>
+        <f t="shared" si="2"/>
+        <v>58.510000000000005</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>59.199999999999996</v>
+        <f t="shared" si="2"/>
+        <v>58.510000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -2101,12 +2976,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2140,7 +3015,7 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2171,7 +3046,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>691.93</v>
@@ -2197,7 +3072,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>10.24</v>
@@ -2223,7 +3098,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>24.44</v>
@@ -2249,7 +3124,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>13.15</v>
@@ -2275,7 +3150,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>2.68</v>
@@ -2301,7 +3176,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>
@@ -2337,11 +3212,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2478,7 +3353,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>
@@ -2502,7 +3377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -2643,7 +3518,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>
@@ -2667,12 +3542,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2722,7 +3597,7 @@
         <v>RMS</v>
       </c>
       <c r="B3">
-        <v>384.822</v>
+        <v>4.665</v>
       </c>
       <c r="C3">
         <v>3.5129999999999999</v>
@@ -2754,11 +3629,11 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <f>SUM(B2:B4)</f>
-        <v>412.72699999999998</v>
+        <v>32.57</v>
       </c>
       <c r="C6">
         <f>SUM(C2:C4)</f>
@@ -2778,7 +3653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -2919,7 +3794,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(B2:B7)</f>

</xml_diff>